<commit_message>
atualização após a 7ª rodada
</commit_message>
<xml_diff>
--- a/matches_FLA2023.xlsx
+++ b/matches_FLA2023.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="matches" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="173">
   <si>
     <t xml:space="preserve">id_match</t>
   </si>
@@ -447,6 +447,15 @@
   </si>
   <si>
     <t xml:space="preserve">2023-05-16 21:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corinthians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campeonato Brasileiro - Round 7</t>
   </si>
   <si>
     <t xml:space="preserve">gols</t>
@@ -537,15 +546,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -605,12 +616,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -631,13 +646,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.18"/>
@@ -645,7 +660,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,6 +1518,32 @@
         <v>141</v>
       </c>
       <c r="H33" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>45067.6666666667</v>
+      </c>
+      <c r="H34" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1522,16 +1563,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.3"/>
   </cols>
   <sheetData>
@@ -1540,10 +1581,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,10 +1592,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,10 +1603,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,10 +1614,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,10 +1625,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,10 +1636,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1606,10 +1647,10 @@
         <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,10 +1658,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,10 +1669,10 @@
         <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,10 +1680,10 @@
         <v>23</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,10 +1691,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1661,10 +1702,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,10 +1713,10 @@
         <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,10 +1724,10 @@
         <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,10 +1735,10 @@
         <v>32</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,10 +1746,10 @@
         <v>37</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,10 +1757,10 @@
         <v>41</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,10 +1768,10 @@
         <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,10 +1779,10 @@
         <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,10 +1790,10 @@
         <v>46</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1760,10 +1801,10 @@
         <v>46</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,10 +1812,10 @@
         <v>46</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,10 +1823,10 @@
         <v>51</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1793,10 +1834,10 @@
         <v>51</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,10 +1845,10 @@
         <v>51</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,10 +1856,10 @@
         <v>55</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1826,10 +1867,10 @@
         <v>55</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,10 +1878,10 @@
         <v>64</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1848,10 +1889,10 @@
         <v>68</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,10 +1900,10 @@
         <v>75</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,10 +1911,10 @@
         <v>79</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,10 +1922,10 @@
         <v>79</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,10 +1933,10 @@
         <v>79</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,10 +1944,10 @@
         <v>82</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,10 +1955,10 @@
         <v>82</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,10 +1966,10 @@
         <v>82</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,10 +1977,10 @@
         <v>85</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1947,10 +1988,10 @@
         <v>85</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,10 +1999,10 @@
         <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1969,10 +2010,10 @@
         <v>93</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,10 +2021,10 @@
         <v>101</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,10 +2032,10 @@
         <v>101</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,10 +2043,10 @@
         <v>101</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2013,10 +2054,10 @@
         <v>105</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,10 +2065,10 @@
         <v>105</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,10 +2076,10 @@
         <v>109</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,10 +2087,10 @@
         <v>114</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2057,10 +2098,10 @@
         <v>114</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2068,10 +2109,10 @@
         <v>114</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,10 +2120,10 @@
         <v>114</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,10 +2131,10 @@
         <v>114</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,10 +2142,10 @@
         <v>114</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,10 +2153,10 @@
         <v>114</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,10 +2164,10 @@
         <v>114</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2134,10 +2175,10 @@
         <v>117</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,10 +2186,10 @@
         <v>117</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2156,10 +2197,10 @@
         <v>120</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2167,10 +2208,10 @@
         <v>125</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,10 +2219,10 @@
         <v>130</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2189,10 +2230,10 @@
         <v>130</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2200,10 +2241,10 @@
         <v>134</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,10 +2252,10 @@
         <v>134</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2222,10 +2263,21 @@
         <v>134</v>
       </c>
       <c r="B63" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="C63" s="0" t="s">
-        <v>152</v>
+      <c r="C64" s="0" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>